<commit_message>
Minor changes and initial state of a new game.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8245A246-E1A5-4041-9AC8-1F0EAD4A5DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D08C88-936B-499F-8094-8B61CA27A598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="73">
   <si>
     <t>Board</t>
   </si>
@@ -106,9 +106,6 @@
     <t>Player(id)</t>
   </si>
   <si>
-    <t>Space(position, occupant)</t>
-  </si>
-  <si>
     <t>Position(x, y)</t>
   </si>
   <si>
@@ -160,9 +157,6 @@
     <t>GetShape()</t>
   </si>
   <si>
-    <t>This would need to change both player1 and player 2</t>
-  </si>
-  <si>
     <t>GetScore()</t>
   </si>
   <si>
@@ -248,6 +242,18 @@
   </si>
   <si>
     <t xml:space="preserve"> +CheckWin()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Space(position, occupant)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Space(position)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -height : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -width : int</t>
   </si>
 </sst>
 </file>
@@ -630,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="B4:W29"/>
+  <dimension ref="B4:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="AA22" sqref="AA22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -641,7 +647,7 @@
     <col min="2" max="2" width="18.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -662,7 +668,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="2:23" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
@@ -685,256 +691,259 @@
       <c r="N5" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="5" t="s">
+      <c r="S5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="W5" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="V5" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L6" t="s">
+      <c r="L6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="W6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="V6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="H7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>12</v>
       </c>
       <c r="N7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="W7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="P7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="V7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>70</v>
-      </c>
-      <c r="H8" t="s">
-        <v>54</v>
+        <v>3</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="N8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="T8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="S8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="L9" t="s">
-        <v>24</v>
+        <v>58</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="N9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.4">
+      <c r="P9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.4">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="B12" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Q11" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H12" t="s">
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="H13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q12" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.4">
-      <c r="H13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="2:23" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B14" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="15" spans="2:23" x14ac:dyDescent="0.4">
+        <v>56</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B15" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:23" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="P16" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="Q17" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.4">
+      <c r="P17" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.4">
       <c r="B18" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B20" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="P26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="Q18" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B22" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B23" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B24" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q24" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B25" s="2" t="s">
+    </row>
+    <row r="27" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
+      <c r="P28" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="B27" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="Q28" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.4">
-      <c r="Q29" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement basic interaction. SwitchTurns() not working properly.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48D3FE3-2D8B-4E3E-8BCF-6AB7580CDDB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC080AEA-3AF0-400A-8425-B088007CA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
   <si>
     <t>Board</t>
   </si>
@@ -52,12 +52,6 @@
     <t>Enum</t>
   </si>
   <si>
-    <t>Player 1</t>
-  </si>
-  <si>
-    <t>Player 2</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t xml:space="preserve"> +Restart()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetCurrentWinner()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -id : int</t>
   </si>
   <si>
@@ -145,9 +136,6 @@
     <t xml:space="preserve"> +SetOccupant(Player)</t>
   </si>
   <si>
-    <t>Occupant</t>
-  </si>
-  <si>
     <t>GetId()</t>
   </si>
   <si>
@@ -274,13 +262,37 @@
     <t xml:space="preserve"> +occupySpace(player, space)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetSpace(position)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +NewGame()</t>
   </si>
   <si>
     <t xml:space="preserve"> +GetUserShapeChoice()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetFreeSpaces() : Spaces[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetSpace(position) : Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +PrintBoard()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetPlayerWithHighestScore() : Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +hasWinner() : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +getWinner() : Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -winner : Player?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -winHistory : Player?[]</t>
+  </si>
+  <si>
+    <t>Winner null = draw</t>
   </si>
 </sst>
 </file>
@@ -304,7 +316,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -314,12 +326,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -336,12 +342,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -663,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="B4:V32"/>
+  <dimension ref="B4:S36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -674,7 +678,7 @@
     <col min="2" max="2" width="18.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -692,12 +696,10 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -715,300 +717,313 @@
         <v>1</v>
       </c>
       <c r="M5" s="1"/>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="P5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.4">
+      <c r="S5" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S6" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="L9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B11" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="S12" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C13" t="s">
+        <v>85</v>
+      </c>
+      <c r="E13" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S13" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B14" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.4">
+      <c r="B16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B9" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="E16" t="s">
+        <v>79</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B19" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="P10" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="P11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B12" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>79</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="V12" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="H13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="V13" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="B15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="P15" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.4">
-      <c r="P16" s="2" t="s">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B20" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="N21" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B24" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B22" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="P22" s="2" t="s">
+      <c r="N24" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="N25" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B23" s="2" t="s">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B27" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="P23" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B24" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="P24" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B25" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B26" t="s">
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B29" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B30" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B31" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B33" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B35" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>45</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B27" t="s">
-        <v>19</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B28" t="s">
-        <v>20</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B29" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B31" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First implementation of CheckWinner().
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC080AEA-3AF0-400A-8425-B088007CA5C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742D788F-93E8-4952-A098-4F1BFBAEB32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>Board</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Shape</t>
   </si>
   <si>
-    <t xml:space="preserve"> -isOccupied : bool</t>
-  </si>
-  <si>
     <t>Player(id, name, score, occupiedSpaces)</t>
   </si>
   <si>
@@ -193,9 +190,6 @@
     <t>SetShape(Shape)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +Game(userShapeChoice)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -userPlayer : Player</t>
   </si>
   <si>
@@ -293,6 +287,24 @@
   </si>
   <si>
     <t>Winner null = draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +PromptPickSpaceToOccupy() : Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +isOccupied : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetBoardSpaceFromInt(int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +ToString() : string</t>
+  </si>
+  <si>
+    <t>ArtificialIntelligence</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +NewTurn()</t>
   </si>
 </sst>
 </file>
@@ -316,7 +328,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +338,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,10 +360,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
@@ -667,10 +686,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="B4:S36"/>
+  <dimension ref="B4:X37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -678,7 +697,7 @@
     <col min="2" max="2" width="18.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -697,7 +716,7 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -721,19 +740,22 @@
         <v>14</v>
       </c>
       <c r="P5" s="1"/>
-      <c r="Q5" s="3" t="s">
+      <c r="Q5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.4">
+        <v>58</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>6</v>
@@ -744,22 +766,22 @@
       <c r="N6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="Q6" s="4" t="s">
         <v>27</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.4">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
@@ -771,19 +793,16 @@
         <v>5</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.4">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="N8" s="2" t="s">
         <v>26</v>
       </c>
@@ -791,14 +810,14 @@
         <v>24</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.4">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="E9" s="5"/>
       <c r="L9" s="2" t="s">
         <v>20</v>
       </c>
@@ -809,117 +828,128 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B12" s="4" t="s">
-        <v>58</v>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B12" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B13" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" t="s">
         <v>83</v>
       </c>
-      <c r="C13" t="s">
-        <v>85</v>
-      </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B14" s="4" t="s">
-        <v>84</v>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B14" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N14" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="E15" t="s">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="N15" s="2" t="s">
+      <c r="H16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.4">
-      <c r="B16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E16" t="s">
-        <v>79</v>
-      </c>
-      <c r="N16" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B17" s="2" t="s">
-        <v>49</v>
+      <c r="E17" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="N17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.4">
+      <c r="B18" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B19" s="2" t="s">
-        <v>67</v>
+        <v>22</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.4">
@@ -927,103 +957,108 @@
         <v>46</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B22" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B24" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B25" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B27" s="2" t="s">
-        <v>57</v>
+      <c r="B27" t="s">
+        <v>40</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B28" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B29" t="s">
-        <v>17</v>
+      <c r="B29" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B30" s="4" t="s">
-        <v>81</v>
+      <c r="B30" s="5" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B31" s="4" t="s">
-        <v>82</v>
+      <c r="B31" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B32" t="s">
-        <v>80</v>
+      <c r="B32" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B34" s="2" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B34" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B36" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B37" s="2" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CheckDraw(). The game now detects when there is a winner or a draw.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742D788F-93E8-4952-A098-4F1BFBAEB32B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D2F4677-FCDB-43FD-9233-7762BE0D5E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t>Board</t>
   </si>
@@ -88,9 +88,6 @@
     <t xml:space="preserve"> -occupiedSpaces : Space[]</t>
   </si>
   <si>
-    <t xml:space="preserve"> +Restart()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -id : int</t>
   </si>
   <si>
@@ -157,9 +154,6 @@
     <t>SetName(string)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +SwitchShape()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +SwitchTurns()</t>
   </si>
   <si>
@@ -220,9 +214,6 @@
     <t xml:space="preserve"> +CheckWin()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +Space(position, occupant)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +Space(position)</t>
   </si>
   <si>
@@ -262,9 +253,6 @@
     <t xml:space="preserve"> +GetUserShapeChoice()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetFreeSpaces() : Spaces[]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +GetSpace(position) : Space</t>
   </si>
   <si>
@@ -305,6 +293,36 @@
   </si>
   <si>
     <t xml:space="preserve"> +NewTurn()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +RestartGame()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -emptySpaces : List&lt;Space&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Space(position : Position, occupant : Player)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetEmptySpaces() : List&lt;Space&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetArrayOfEmptySpacesForBoard(boardHeight : int, boardWidth : int) : Space[]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Board(spaces : Spaces[])</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Board()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetEmptySpaces(emptySpaces : List&lt;Space&gt;)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +CheckGameResult()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +CheckDraw()</t>
   </si>
 </sst>
 </file>
@@ -689,7 +707,7 @@
   <dimension ref="B4:X37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -744,10 +762,10 @@
         <v>4</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.4">
@@ -755,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>6</v>
@@ -764,13 +782,13 @@
         <v>9</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.4">
@@ -778,62 +796,64 @@
         <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="L9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N9" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="N10" s="2" t="s">
         <v>16</v>
@@ -841,224 +861,239 @@
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B13" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
+        <v>79</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>8</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E14" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.4">
+      <c r="E15" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.4">
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="16" spans="2:24" x14ac:dyDescent="0.4">
       <c r="B16" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.4">
       <c r="E17" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B18" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B19" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B20" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B22" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B24" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B25" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
-        <v>40</v>
+        <v>86</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B28" t="s">
-        <v>17</v>
+      <c r="B28" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B29" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B30" s="5" t="s">
-        <v>80</v>
+      <c r="B30" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.4">
-      <c r="B31" t="s">
-        <v>78</v>
+      <c r="B31" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.4">
       <c r="B32" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B33" s="2" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B34" s="2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B35" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B36" t="s">
-        <v>44</v>
+      <c r="B36" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.4">
       <c r="B37" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add diplay of results and allow playing again. Bug: Choosing shape O for user misbehaves.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A399AE61-3B61-4C22-8EA7-2DD06B2A7439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C201CC2-613D-44FA-BA50-33B5F205F2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Board</t>
   </si>
@@ -85,9 +85,6 @@
     <t xml:space="preserve"> -score : int</t>
   </si>
   <si>
-    <t xml:space="preserve"> -occupiedSpaces : Space[]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -id : int</t>
   </si>
   <si>
@@ -323,13 +320,40 @@
   </si>
   <si>
     <t xml:space="preserve"> +GetConsecutiveShapesToWin() : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +AddToOccupiedSpaces(space : Space)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -gameIsOver : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetGameIsOver() : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetGameIsOver(gameIsOver : bool)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -occupiedSpaces : List&lt;Space&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetOccupiedSpaces() : List&lt;Space&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +ResetOccupiedSpaces()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +DisplayPlayersScore()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +DisplayWinner(Player?)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -339,7 +363,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -381,10 +412,10 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,32 +735,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="A1:R34"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.4609375" customWidth="1"/>
-    <col min="3" max="3" width="45.4609375" customWidth="1"/>
-    <col min="4" max="4" width="5.23046875" customWidth="1"/>
-    <col min="5" max="5" width="38.61328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.61328125" customWidth="1"/>
-    <col min="7" max="7" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3.23046875" customWidth="1"/>
-    <col min="9" max="9" width="33.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.15234375" customWidth="1"/>
-    <col min="11" max="11" width="6.921875" customWidth="1"/>
-    <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="40" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.921875" customWidth="1"/>
-    <col min="15" max="15" width="4.921875" customWidth="1"/>
+    <col min="1" max="1" width="29.69140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3.61328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.4609375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="2.84375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.07421875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.61328125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.23046875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="33.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.15234375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="6.921875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="3" style="2" customWidth="1"/>
+    <col min="13" max="13" width="40" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2.921875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="4.921875" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -749,348 +781,382 @@
       <c r="I1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C13" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="I14" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="R4" s="1"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" s="2" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="C12" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A17" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A19" s="2" t="s">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A21" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A22" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A24" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A27" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A28" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A29" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A30" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A31" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A32" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A33" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A34" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor adjustments to previous bug fix and update UML.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C201CC2-613D-44FA-BA50-33B5F205F2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65981BA8-D4F6-4881-A8BA-578F4213F87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>Board</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Player</t>
   </si>
   <si>
-    <t xml:space="preserve"> -score : int</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -id : int</t>
   </si>
   <si>
@@ -274,12 +271,6 @@
     <t xml:space="preserve"> +PromptPlayAgain() : bool</t>
   </si>
   <si>
-    <t xml:space="preserve"> +Player(id, name, score, occupiedSpaces)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +Player(id, name, score)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +Player(id, name)</t>
   </si>
   <si>
@@ -301,18 +292,12 @@
     <t xml:space="preserve"> +SetShape(Shape)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetScore()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +GetHasTurn()</t>
   </si>
   <si>
     <t xml:space="preserve"> +SetHasTurn(hasTurn)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +SetScore(int)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +GetBoardDimensions() : (int height, int width)</t>
   </si>
   <si>
@@ -347,6 +332,15 @@
   </si>
   <si>
     <t xml:space="preserve"> +DisplayWinner(Player?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -userScore : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -botScore : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Player(id, name, occupiedSpaces)</t>
   </si>
 </sst>
 </file>
@@ -409,13 +403,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="A1:R39"/>
+  <dimension ref="A1:R41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -785,10 +780,10 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -796,7 +791,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -805,13 +800,13 @@
         <v>9</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -819,344 +814,358 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" s="6"/>
       <c r="I4" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>66</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H5" s="6"/>
       <c r="I5" s="4" t="s">
-        <v>15</v>
+        <v>94</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>99</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="H6" s="6"/>
       <c r="I6" s="4" t="s">
-        <v>99</v>
+        <v>25</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="4" t="s">
-        <v>26</v>
-      </c>
+      <c r="H7" s="6"/>
       <c r="M7" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>77</v>
+        <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="4" t="s">
+        <v>101</v>
+      </c>
       <c r="M8" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
-        <v>57</v>
+      <c r="A9" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H9" s="6"/>
       <c r="I9" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>59</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="H10" s="6"/>
       <c r="I10" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="4" t="s">
         <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>74</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H12" s="6"/>
       <c r="I12" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="6"/>
+      <c r="I13" s="4" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="C13" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>34</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="H14" s="6"/>
       <c r="I14" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="6"/>
+      <c r="I15" s="4" t="s">
         <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>52</v>
+      </c>
+      <c r="H16" s="6"/>
       <c r="I16" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>60</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="H17" s="6"/>
       <c r="I17" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H18" s="6"/>
       <c r="I18" s="4" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>27</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="H19" s="6"/>
       <c r="I19" s="4" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>90</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>100</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>101</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>50</v>
+      <c r="A30" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
-        <v>102</v>
+      <c r="A38" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="4" t="s">
-        <v>30</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validate if chosen space is occupied inside PromptPickSpaceToOccupy() instead of validating it in NewTurn().
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65981BA8-D4F6-4881-A8BA-578F4213F87F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516AF907-4A6C-4600-A1C3-C7BE526C5931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Board</t>
   </si>
@@ -157,9 +157,6 @@
     <t>Rule</t>
   </si>
   <si>
-    <t xml:space="preserve"> +Reset()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +Space(position)</t>
   </si>
   <si>
@@ -196,18 +193,6 @@
     <t xml:space="preserve"> +PrintBoard()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetPlayerWithHighestScore() : Player</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +hasWinner() : bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +getWinner() : Player</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -winner : Player?</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +PromptPickSpaceToOccupy() : Space</t>
   </si>
   <si>
@@ -220,7 +205,7 @@
     <t xml:space="preserve"> +ToString() : string</t>
   </si>
   <si>
-    <t>ArtificialIntelligence</t>
+    <t>BotArtificialIntelligence</t>
   </si>
   <si>
     <t xml:space="preserve"> +NewTurn()</t>
@@ -341,6 +326,9 @@
   </si>
   <si>
     <t xml:space="preserve"> +Player(id, name, occupiedSpaces)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetMove()</t>
   </si>
 </sst>
 </file>
@@ -371,7 +359,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,12 +369,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,13 +385,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -730,10 +711,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="A1:R41"/>
+  <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -752,8 +733,8 @@
     <col min="12" max="12" width="3" style="2" customWidth="1"/>
     <col min="13" max="13" width="40" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.921875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="4.921875" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="9.23046875" style="2"/>
+    <col min="15" max="17" width="18.3828125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.23046875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
@@ -783,7 +764,7 @@
         <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -791,7 +772,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -806,7 +787,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -814,7 +795,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>32</v>
@@ -829,7 +810,7 @@
         <v>5</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
@@ -839,7 +820,7 @@
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4" t="s">
         <v>22</v>
       </c>
@@ -847,7 +828,7 @@
         <v>20</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R4" s="1"/>
     </row>
@@ -856,50 +837,53 @@
         <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="O5" s="2" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="H6" s="5"/>
       <c r="I6" s="4" t="s">
         <v>25</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
       <c r="M7" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
@@ -907,17 +891,17 @@
         <v>17</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -925,144 +909,141 @@
         <v>27</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="4" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="H10" s="5"/>
       <c r="I10" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A11" s="5" t="s">
-        <v>56</v>
+      <c r="A11" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="H12" s="6"/>
+        <v>68</v>
+      </c>
+      <c r="H12" s="5"/>
       <c r="I12" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="H13" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="H13" s="5"/>
       <c r="I13" s="4" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="6"/>
+      <c r="C14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H14" s="5"/>
       <c r="I14" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
       <c r="I15" s="4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="H16" s="5"/>
       <c r="I16" s="4" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H17" s="6"/>
+        <v>18</v>
+      </c>
+      <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I21" s="4" t="s">
         <v>29</v>
@@ -1070,52 +1051,52 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>38</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>93</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>54</v>
+      <c r="A28" s="4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>55</v>
+      <c r="A29" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
-        <v>53</v>
+      <c r="A30" s="4" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1125,46 +1106,26 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" s="4" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored the game to use an enum GameResult to determine terminal states.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516AF907-4A6C-4600-A1C3-C7BE526C5931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E2D645-038A-4936-B410-B9F5DBFAF7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
   <si>
     <t>Board</t>
   </si>
@@ -196,9 +196,6 @@
     <t xml:space="preserve"> +PromptPickSpaceToOccupy() : Space</t>
   </si>
   <si>
-    <t xml:space="preserve"> +isOccupied : bool</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +GetBoardSpaceFromInt(int)</t>
   </si>
   <si>
@@ -238,18 +235,12 @@
     <t xml:space="preserve"> +CheckGameResult()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +CheckDraw() : bool</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +CheckWin() : (hasWinner : bool, winner : Player?)</t>
   </si>
   <si>
     <t xml:space="preserve"> -winHistory : List&lt;Player?&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve"> -drawCount : int</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -turnCount : int</t>
   </si>
   <si>
@@ -329,6 +320,42 @@
   </si>
   <si>
     <t xml:space="preserve"> +GetMove()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +IsOccupied : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetSpaces()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetSpaces(spaces : Space[])</t>
+  </si>
+  <si>
+    <t>BoardState</t>
+  </si>
+  <si>
+    <t>Incomplete</t>
+  </si>
+  <si>
+    <t>WinnerX</t>
+  </si>
+  <si>
+    <t>Winner0</t>
+  </si>
+  <si>
+    <t>Tie</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetResult()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +CheckTie() : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -tieScore : int</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -boardState : GameResult</t>
   </si>
 </sst>
 </file>
@@ -359,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -369,6 +396,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,13 +418,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
   <dimension ref="A1:R37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -725,9 +759,9 @@
     <col min="4" max="4" width="2.84375" style="2" customWidth="1"/>
     <col min="5" max="5" width="28.07421875" style="2" customWidth="1"/>
     <col min="6" max="6" width="3.61328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.3828125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.765625" style="2" customWidth="1"/>
     <col min="8" max="8" width="3.23046875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="33.84375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.921875" style="2" customWidth="1"/>
     <col min="10" max="10" width="3.15234375" style="2" customWidth="1"/>
     <col min="11" max="11" width="6.921875" style="2" customWidth="1"/>
     <col min="12" max="12" width="3" style="2" customWidth="1"/>
@@ -764,7 +798,7 @@
         <v>39</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -837,28 +871,31 @@
         <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>106</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>40</v>
@@ -868,183 +905,195 @@
         <v>25</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="5"/>
       <c r="M7" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>71</v>
+        <v>27</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>53</v>
+        <v>95</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>51</v>
+      <c r="C15" s="6" t="s">
+        <v>66</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="4" t="s">
-        <v>54</v>
+      <c r="C16" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
       <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
+      <c r="C19" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="I20" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>28</v>
       </c>
+      <c r="C21" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="I21" s="4" t="s">
         <v>29</v>
       </c>
@@ -1065,38 +1114,56 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
-        <v>87</v>
+      <c r="A25" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="4" t="s">
-        <v>88</v>
+      <c r="A26" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="C27" s="4" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="6" t="s">
         <v>48</v>
       </c>
+      <c r="C28" s="4" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
         <v>57</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="4" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
@@ -1110,18 +1177,18 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>72</v>
+      <c r="A34" s="6" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>93</v>
+      <c r="A35" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Cleanup unnecessary code and comments.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E2D645-038A-4936-B410-B9F5DBFAF7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C32108-CDAA-4138-AF6D-00799D2C44AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
   <si>
     <t>Board</t>
   </si>
@@ -112,12 +112,6 @@
     <t xml:space="preserve"> +SetOccupant(Player)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -HasTurn : bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +SwitchTurns()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -currentTurnPlayer : Player</t>
   </si>
   <si>
@@ -232,9 +226,6 @@
     <t xml:space="preserve"> +SetEmptySpaces(emptySpaces : List&lt;Space&gt;)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +CheckGameResult()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +CheckWin() : (hasWinner : bool, winner : Player?)</t>
   </si>
   <si>
@@ -268,12 +259,6 @@
     <t xml:space="preserve"> +SetShape(Shape)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetHasTurn()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +SetHasTurn(hasTurn)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +GetBoardDimensions() : (int height, int width)</t>
   </si>
   <si>
@@ -289,12 +274,6 @@
     <t xml:space="preserve"> -gameIsOver : bool</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetGameIsOver() : bool</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +SetGameIsOver(gameIsOver : bool)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -occupiedSpaces : List&lt;Space&gt;</t>
   </si>
   <si>
@@ -307,9 +286,6 @@
     <t xml:space="preserve"> +DisplayPlayersScore()</t>
   </si>
   <si>
-    <t xml:space="preserve"> +DisplayWinner(Player?)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -userScore : int</t>
   </si>
   <si>
@@ -355,14 +331,41 @@
     <t xml:space="preserve"> -tieScore : int</t>
   </si>
   <si>
-    <t xml:space="preserve"> -boardState : GameResult</t>
+    <t xml:space="preserve"> -result : GameResult</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetResult()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetPlayerFromShape(shape : Shape) : Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +DisplayWinner(gameResult : GameResult)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetPlayerFromResult(result : GameResult) : Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +UpdateScores(result : GameResult)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetResultFromBoard(board)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetShapeOfTurnFromBoard(Board board) : Shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +HasTurn(board : Board) : bool</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +DetermineTurn()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -385,8 +388,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -396,12 +407,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -425,7 +430,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -748,7 +753,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -795,10 +800,10 @@
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
@@ -806,7 +811,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
@@ -821,7 +826,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
@@ -829,10 +834,10 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -844,12 +849,12 @@
         <v>5</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
@@ -862,80 +867,80 @@
         <v>20</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>21</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>106</v>
+        <v>83</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="4" t="s">
-        <v>25</v>
-      </c>
       <c r="M6" s="4" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="H7" s="5"/>
+      <c r="I7" s="4" t="s">
+        <v>85</v>
+      </c>
       <c r="M7" s="4" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>8</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
@@ -943,101 +948,101 @@
         <v>17</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>24</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>66</v>
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>63</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="4" t="s">
-        <v>76</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>104</v>
+        <v>41</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>96</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="4" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1045,155 +1050,158 @@
         <v>18</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>88</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>82</v>
+      <c r="C20" s="6" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>29</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>4</v>
+      <c r="A25" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>98</v>
+      <c r="A26" s="4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A28" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="C30" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>57</v>
+      <c r="A31" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>49</v>
+      <c r="A32" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>52</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>69</v>
+      <c r="A34" s="4" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
-        <v>90</v>
+      <c r="A35" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement artificial intelligence for bot using minimax algorithm.
</commit_message>
<xml_diff>
--- a/UML_TicTacToe.xlsx
+++ b/UML_TicTacToe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\development\c#\TicTacToe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C32108-CDAA-4138-AF6D-00799D2C44AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697AF641-0D1A-4AEE-9955-1EF865DF86F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-30828" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{76BE3D13-E20F-4EB2-A36F-CB94B6DBFA67}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="118">
   <si>
     <t>Board</t>
   </si>
@@ -58,12 +58,6 @@
     <t xml:space="preserve"> -position : Position [readonly]</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetPosition()</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> +GetOccupant()</t>
-  </si>
-  <si>
     <t>x : int</t>
   </si>
   <si>
@@ -127,9 +121,6 @@
     <t xml:space="preserve"> +SetCurrentTurnPlayer(Player)</t>
   </si>
   <si>
-    <t xml:space="preserve"> -occupant : Player [nullable]</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +Game()</t>
   </si>
   <si>
@@ -172,9 +163,6 @@
     <t xml:space="preserve"> -consecutiveShapesToWin</t>
   </si>
   <si>
-    <t xml:space="preserve"> +occupySpace(player, space)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +NewGame()</t>
   </si>
   <si>
@@ -196,9 +184,6 @@
     <t xml:space="preserve"> +ToString() : string</t>
   </si>
   <si>
-    <t>BotArtificialIntelligence</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +NewTurn()</t>
   </si>
   <si>
@@ -226,9 +211,6 @@
     <t xml:space="preserve"> +SetEmptySpaces(emptySpaces : List&lt;Space&gt;)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +CheckWin() : (hasWinner : bool, winner : Player?)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> -winHistory : List&lt;Player?&gt;</t>
   </si>
   <si>
@@ -295,9 +277,6 @@
     <t xml:space="preserve"> +Player(id, name, occupiedSpaces)</t>
   </si>
   <si>
-    <t xml:space="preserve"> +GetMove()</t>
-  </si>
-  <si>
     <t xml:space="preserve"> +IsOccupied : bool</t>
   </si>
   <si>
@@ -359,13 +338,64 @@
   </si>
   <si>
     <t xml:space="preserve"> +DetermineTurn()</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetOccupant() : Player</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetPosition() : Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +OccupySpace(board : Board, space Space)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +OccupySpace(board : Board, space Space, player : Player?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +CheckWin() : (hasWinner : bool, winner : Shape?)</t>
+  </si>
+  <si>
+    <t>BotAI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetBoard(board : Board)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Game(board : Board)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetBoardClone(Board) : Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -occupant : Shape?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetSpaceClone(Space) : Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +SetSpace(space : Space)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetBoardSpaceFromCoordinates(x : int, y : int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetRandomMove(board Board) : Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetMinimaxMove(board : Board) : Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +Minimax(board : Board, isMaximizing : bool) : int, Space</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> +GetScore(board : Board) : int</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +422,13 @@
       <i/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -431,6 +468,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96DA328-D30C-4104-AA24-BB92042EC0B8}">
-  <dimension ref="A1:R37"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="O2" sqref="O2:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.9" x14ac:dyDescent="0.35"/>
@@ -778,7 +816,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -794,414 +832,446 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>110</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O5" s="2" t="s">
-        <v>86</v>
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H6" s="5"/>
       <c r="M6" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>7</v>
+        <v>102</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="4" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>8</v>
+        <v>101</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="4" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="4" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>111</v>
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>63</v>
+      <c r="A15" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="4" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>96</v>
+        <v>28</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="4" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>48</v>
+        <v>105</v>
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>104</v>
+      <c r="C20" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>95</v>
+        <v>27</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>99</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>27</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>32</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>90</v>
+        <v>49</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>55</v>
+        <v>96</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>91</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>92</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="C36" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>27</v>
+        <v>95</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>